<commit_message>
tests: make car case consistent
</commit_message>
<xml_diff>
--- a/tests/data/_schema/physical/car_dms_rules.xlsx
+++ b/tests/data/_schema/physical/car_dms_rules.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikola/Repos/neat/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndersAlbert\Projects\internal\neat\tests\data\_schema\physical\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C9B0377-3EB0-DB48-BF15-23129165799D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C0183F2-89D4-405F-A5B8-F4EBF70D3875}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="42700" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -132,9 +132,6 @@
     <t>make</t>
   </si>
   <si>
-    <t>edge(type=Car.Manufacturer)</t>
-  </si>
-  <si>
     <t>Manufacturer</t>
   </si>
   <si>
@@ -228,9 +225,6 @@
     <t>http://purl.org/cognite/neat/data-model/verified/logical/sp_example_car/CarModel/1/Manufacturer/name</t>
   </si>
   <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/sp_example_car/CarModel/1/Car/Car.Manufacturer</t>
-  </si>
-  <si>
     <t>http://purl.org/cognite/neat/data-model/verified/logical/sp_example_car/CarModel/1/Car/color</t>
   </si>
   <si>
@@ -244,6 +238,12 @@
   </si>
   <si>
     <t>http://purl.org/cognite/neat/data-model/verified/logical/sp_example_car/CarModel/1/Color</t>
+  </si>
+  <si>
+    <t>edge(type=make)</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/logical/sp_example_car/CarModel/1/Car/make</t>
   </si>
 </sst>
 </file>
@@ -253,7 +253,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -279,6 +279,14 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -302,10 +310,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -314,8 +323,10 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -618,15 +629,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView zoomScale="285" workbookViewId="0"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="26.5" customWidth="1"/>
+    <col min="2" max="2" width="26.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -634,7 +647,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -642,7 +655,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -650,7 +663,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -658,17 +671,17 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -676,7 +689,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
@@ -684,7 +697,7 @@
         <v>45695.809878616063</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
@@ -692,12 +705,12 @@
         <v>45695.809878616303</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
@@ -711,26 +724,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P7"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O1" sqref="O1"/>
+      <selection pane="bottomLeft" activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.5" customWidth="1"/>
-    <col min="2" max="2" width="13.5" customWidth="1"/>
+    <col min="1" max="1" width="34.44140625" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" customWidth="1"/>
     <col min="3" max="4" width="13" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="27.5" customWidth="1"/>
+    <col min="5" max="5" width="27.44140625" customWidth="1"/>
     <col min="6" max="6" width="13" customWidth="1"/>
     <col min="7" max="11" width="13" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="18.5" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="18.44140625" hidden="1" customWidth="1"/>
     <col min="13" max="14" width="13" hidden="1" customWidth="1"/>
     <col min="15" max="15" width="94.6640625" customWidth="1"/>
     <col min="16" max="16" width="70" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A1" s="3" t="s">
         <v>16</v>
       </c>
@@ -749,7 +762,7 @@
       <c r="N1" s="4"/>
       <c r="O1" s="4"/>
     </row>
-    <row r="2" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>17</v>
       </c>
@@ -799,7 +812,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -807,30 +820,30 @@
         <v>34</v>
       </c>
       <c r="E3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F3" t="s">
         <v>35</v>
-      </c>
-      <c r="F3" t="s">
-        <v>36</v>
       </c>
       <c r="I3" t="b">
         <v>1</v>
       </c>
-      <c r="O3" t="s">
-        <v>67</v>
+      <c r="O3" s="6" t="s">
+        <v>72</v>
       </c>
       <c r="P3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>33</v>
       </c>
       <c r="B4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" t="s">
         <v>38</v>
-      </c>
-      <c r="F4" t="s">
-        <v>39</v>
       </c>
       <c r="G4" t="b">
         <v>1</v>
@@ -845,27 +858,27 @@
         <v>33</v>
       </c>
       <c r="L4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="P4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>33</v>
       </c>
       <c r="B5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" t="s">
         <v>41</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>42</v>
-      </c>
-      <c r="F5" t="s">
-        <v>43</v>
       </c>
       <c r="G5" t="b">
         <v>1</v>
@@ -880,24 +893,24 @@
         <v>33</v>
       </c>
       <c r="L5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="P5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
       </c>
       <c r="F6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G6" t="b">
         <v>1</v>
@@ -909,27 +922,27 @@
         <v>0</v>
       </c>
       <c r="K6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L6" t="s">
         <v>8</v>
       </c>
       <c r="O6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="P6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
       </c>
       <c r="F7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G7" t="b">
         <v>1</v>
@@ -941,19 +954,22 @@
         <v>0</v>
       </c>
       <c r="K7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L7" t="s">
         <v>8</v>
       </c>
       <c r="O7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="P7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="O3" r:id="rId1" xr:uid="{97E13F1D-51F0-49F2-A941-AE90CC7E29C2}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -962,21 +978,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H18" sqref="H18"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.5" customWidth="1"/>
+    <col min="1" max="1" width="19.44140625" customWidth="1"/>
     <col min="2" max="7" width="13" customWidth="1"/>
     <col min="8" max="8" width="70" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A1" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -986,7 +1002,7 @@
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
     </row>
-    <row r="2" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>17</v>
       </c>
@@ -997,13 +1013,13 @@
         <v>20</v>
       </c>
       <c r="D2" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>50</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>51</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>31</v>
@@ -1012,7 +1028,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -1020,38 +1036,38 @@
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F4" t="b">
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F5" t="b">
         <v>1</v>
       </c>
       <c r="G5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1068,16 +1084,16 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.5" customWidth="1"/>
+    <col min="1" max="1" width="24.44140625" customWidth="1"/>
     <col min="2" max="5" width="13" customWidth="1"/>
     <col min="6" max="6" width="13" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A1" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -1085,7 +1101,7 @@
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
     </row>
-    <row r="2" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>27</v>
       </c>
@@ -1099,25 +1115,25 @@
         <v>30</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1134,28 +1150,28 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.5" customWidth="1"/>
+    <col min="1" max="1" width="30.44140625" customWidth="1"/>
     <col min="2" max="4" width="13" customWidth="1"/>
     <col min="5" max="5" width="13" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A1" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
     </row>
-    <row r="2" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>58</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>59</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>19</v>
@@ -1181,28 +1197,28 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.5" customWidth="1"/>
+    <col min="1" max="1" width="19.44140625" customWidth="1"/>
     <col min="2" max="4" width="13" customWidth="1"/>
     <col min="5" max="5" width="13" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A1" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
     </row>
-    <row r="2" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>61</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>62</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>19</v>
@@ -1214,12 +1230,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" t="s">
         <v>63</v>
-      </c>
-      <c r="B3" t="s">
-        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
🚗 Car Example consistent (#1185)
# Description

The care example has triples, conceptual and DMS models. They were not
entirely consistent, so when inferring model from the triples there were
inconsistencies.

## Bump

- [ ] Patch
- [ ] Minor
- [x] Skip
</commit_message>
<xml_diff>
--- a/tests/data/_schema/physical/car_dms_rules.xlsx
+++ b/tests/data/_schema/physical/car_dms_rules.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikola/Repos/neat/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndersAlbert\Projects\internal\neat\tests\data\_schema\physical\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C9B0377-3EB0-DB48-BF15-23129165799D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C0183F2-89D4-405F-A5B8-F4EBF70D3875}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="42700" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -132,9 +132,6 @@
     <t>make</t>
   </si>
   <si>
-    <t>edge(type=Car.Manufacturer)</t>
-  </si>
-  <si>
     <t>Manufacturer</t>
   </si>
   <si>
@@ -228,9 +225,6 @@
     <t>http://purl.org/cognite/neat/data-model/verified/logical/sp_example_car/CarModel/1/Manufacturer/name</t>
   </si>
   <si>
-    <t>http://purl.org/cognite/neat/data-model/verified/logical/sp_example_car/CarModel/1/Car/Car.Manufacturer</t>
-  </si>
-  <si>
     <t>http://purl.org/cognite/neat/data-model/verified/logical/sp_example_car/CarModel/1/Car/color</t>
   </si>
   <si>
@@ -244,6 +238,12 @@
   </si>
   <si>
     <t>http://purl.org/cognite/neat/data-model/verified/logical/sp_example_car/CarModel/1/Color</t>
+  </si>
+  <si>
+    <t>edge(type=make)</t>
+  </si>
+  <si>
+    <t>http://purl.org/cognite/neat/data-model/verified/logical/sp_example_car/CarModel/1/Car/make</t>
   </si>
 </sst>
 </file>
@@ -253,7 +253,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -279,6 +279,14 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -302,10 +310,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -314,8 +323,10 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -618,15 +629,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView zoomScale="285" workbookViewId="0"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="26.5" customWidth="1"/>
+    <col min="2" max="2" width="26.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -634,7 +647,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -642,7 +655,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -650,7 +663,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -658,17 +671,17 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -676,7 +689,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
@@ -684,7 +697,7 @@
         <v>45695.809878616063</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
@@ -692,12 +705,12 @@
         <v>45695.809878616303</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
@@ -711,26 +724,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P7"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O1" sqref="O1"/>
+      <selection pane="bottomLeft" activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.5" customWidth="1"/>
-    <col min="2" max="2" width="13.5" customWidth="1"/>
+    <col min="1" max="1" width="34.44140625" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" customWidth="1"/>
     <col min="3" max="4" width="13" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="27.5" customWidth="1"/>
+    <col min="5" max="5" width="27.44140625" customWidth="1"/>
     <col min="6" max="6" width="13" customWidth="1"/>
     <col min="7" max="11" width="13" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="18.5" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="18.44140625" hidden="1" customWidth="1"/>
     <col min="13" max="14" width="13" hidden="1" customWidth="1"/>
     <col min="15" max="15" width="94.6640625" customWidth="1"/>
     <col min="16" max="16" width="70" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A1" s="3" t="s">
         <v>16</v>
       </c>
@@ -749,7 +762,7 @@
       <c r="N1" s="4"/>
       <c r="O1" s="4"/>
     </row>
-    <row r="2" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>17</v>
       </c>
@@ -799,7 +812,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -807,30 +820,30 @@
         <v>34</v>
       </c>
       <c r="E3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F3" t="s">
         <v>35</v>
-      </c>
-      <c r="F3" t="s">
-        <v>36</v>
       </c>
       <c r="I3" t="b">
         <v>1</v>
       </c>
-      <c r="O3" t="s">
-        <v>67</v>
+      <c r="O3" s="6" t="s">
+        <v>72</v>
       </c>
       <c r="P3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>33</v>
       </c>
       <c r="B4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" t="s">
         <v>38</v>
-      </c>
-      <c r="F4" t="s">
-        <v>39</v>
       </c>
       <c r="G4" t="b">
         <v>1</v>
@@ -845,27 +858,27 @@
         <v>33</v>
       </c>
       <c r="L4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="P4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>33</v>
       </c>
       <c r="B5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" t="s">
         <v>41</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>42</v>
-      </c>
-      <c r="F5" t="s">
-        <v>43</v>
       </c>
       <c r="G5" t="b">
         <v>1</v>
@@ -880,24 +893,24 @@
         <v>33</v>
       </c>
       <c r="L5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="P5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
       </c>
       <c r="F6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G6" t="b">
         <v>1</v>
@@ -909,27 +922,27 @@
         <v>0</v>
       </c>
       <c r="K6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L6" t="s">
         <v>8</v>
       </c>
       <c r="O6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="P6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
       </c>
       <c r="F7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G7" t="b">
         <v>1</v>
@@ -941,19 +954,22 @@
         <v>0</v>
       </c>
       <c r="K7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L7" t="s">
         <v>8</v>
       </c>
       <c r="O7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="P7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="O3" r:id="rId1" xr:uid="{97E13F1D-51F0-49F2-A941-AE90CC7E29C2}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -962,21 +978,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H18" sqref="H18"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.5" customWidth="1"/>
+    <col min="1" max="1" width="19.44140625" customWidth="1"/>
     <col min="2" max="7" width="13" customWidth="1"/>
     <col min="8" max="8" width="70" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A1" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -986,7 +1002,7 @@
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
     </row>
-    <row r="2" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>17</v>
       </c>
@@ -997,13 +1013,13 @@
         <v>20</v>
       </c>
       <c r="D2" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>50</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>51</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>31</v>
@@ -1012,7 +1028,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -1020,38 +1036,38 @@
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F4" t="b">
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F5" t="b">
         <v>1</v>
       </c>
       <c r="G5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1068,16 +1084,16 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.5" customWidth="1"/>
+    <col min="1" max="1" width="24.44140625" customWidth="1"/>
     <col min="2" max="5" width="13" customWidth="1"/>
     <col min="6" max="6" width="13" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A1" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -1085,7 +1101,7 @@
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
     </row>
-    <row r="2" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>27</v>
       </c>
@@ -1099,25 +1115,25 @@
         <v>30</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1134,28 +1150,28 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.5" customWidth="1"/>
+    <col min="1" max="1" width="30.44140625" customWidth="1"/>
     <col min="2" max="4" width="13" customWidth="1"/>
     <col min="5" max="5" width="13" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A1" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
     </row>
-    <row r="2" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>58</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>59</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>19</v>
@@ -1181,28 +1197,28 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.5" customWidth="1"/>
+    <col min="1" max="1" width="19.44140625" customWidth="1"/>
     <col min="2" max="4" width="13" customWidth="1"/>
     <col min="5" max="5" width="13" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A1" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
     </row>
-    <row r="2" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>61</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>62</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>19</v>
@@ -1214,12 +1230,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" t="s">
         <v>63</v>
-      </c>
-      <c r="B3" t="s">
-        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: test_load_car_example, renaming of logical with conceptual in test data
</commit_message>
<xml_diff>
--- a/tests/data/_schema/physical/car_dms_rules.xlsx
+++ b/tests/data/_schema/physical/car_dms_rules.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikola/Repos/neat/tests/data/_schema/physical/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DD1EA16-D174-8D4E-83E4-990FACD0DC4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F87C31E1-F3AA-7549-8BB1-7B9DC6D96D2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="42700" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="42700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -72,9 +72,6 @@
     <t>sourceId</t>
   </si>
   <si>
-    <t>logical</t>
-  </si>
-  <si>
     <t>Definition of Properties per Class</t>
   </si>
   <si>
@@ -120,9 +117,6 @@
     <t>Constraint</t>
   </si>
   <si>
-    <t>Logical</t>
-  </si>
-  <si>
     <t>Neat ID</t>
   </si>
   <si>
@@ -244,6 +238,12 @@
   </si>
   <si>
     <t>http://purl.org/cognite/neat/data-model/verified/conceptual/sp_example_car/CarModel/1/Color/name</t>
+  </si>
+  <si>
+    <t>Conceptual</t>
+  </si>
+  <si>
+    <t>conceptual</t>
   </si>
 </sst>
 </file>
@@ -625,7 +625,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView zoomScale="285" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="285" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -706,7 +708,7 @@
     </row>
     <row r="11" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>15</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -718,9 +720,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+    <sheetView zoomScale="125" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O3" sqref="O3:O7"/>
+      <selection pane="bottomLeft" activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -739,7 +741,7 @@
   <sheetData>
     <row r="1" spans="1:16" ht="26" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -758,86 +760,86 @@
     </row>
     <row r="2" spans="1:16" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="I2" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="J2" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="K2" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="L2" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="M2" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="N2" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="O2" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="P2" s="5" t="s">
         <v>30</v>
-      </c>
-      <c r="O2" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="P2" s="5" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" t="s">
         <v>33</v>
       </c>
-      <c r="B3" t="s">
+      <c r="F3" t="s">
         <v>34</v>
-      </c>
-      <c r="E3" t="s">
-        <v>35</v>
-      </c>
-      <c r="F3" t="s">
-        <v>36</v>
       </c>
       <c r="I3" t="b">
         <v>1</v>
       </c>
       <c r="O3" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="P3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G4" t="b">
         <v>1</v>
@@ -849,30 +851,30 @@
         <v>0</v>
       </c>
       <c r="K4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="L4" t="s">
+        <v>36</v>
+      </c>
+      <c r="O4" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="P4" t="s">
         <v>38</v>
-      </c>
-      <c r="O4" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="P4" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" t="s">
         <v>41</v>
-      </c>
-      <c r="E5" t="s">
-        <v>42</v>
-      </c>
-      <c r="F5" t="s">
-        <v>43</v>
       </c>
       <c r="G5" t="b">
         <v>1</v>
@@ -884,27 +886,27 @@
         <v>0</v>
       </c>
       <c r="K5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="L5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="O5" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="P5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
       </c>
       <c r="F6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G6" t="b">
         <v>1</v>
@@ -916,27 +918,27 @@
         <v>0</v>
       </c>
       <c r="K6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="L6" t="s">
         <v>8</v>
       </c>
       <c r="O6" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="P6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
       </c>
       <c r="F7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G7" t="b">
         <v>1</v>
@@ -948,16 +950,16 @@
         <v>0</v>
       </c>
       <c r="K7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="L7" t="s">
         <v>8</v>
       </c>
       <c r="O7" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="P7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -972,7 +974,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G3" sqref="G3:G5"/>
+      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -985,7 +987,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="26" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -997,70 +999,70 @@
     </row>
     <row r="2" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>20</v>
-      </c>
       <c r="D2" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>51</v>
-      </c>
       <c r="G2" s="5" t="s">
-        <v>31</v>
+        <v>71</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F3" t="b">
         <v>1</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F4" t="b">
         <v>1</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F5" t="b">
         <v>1</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1086,7 +1088,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="26" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -1096,37 +1098,37 @@
     </row>
     <row r="2" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>20</v>
-      </c>
       <c r="D2" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>30</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1152,7 +1154,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="26" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -1161,19 +1163,19 @@
     </row>
     <row r="2" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>20</v>
-      </c>
       <c r="E2" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1199,7 +1201,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="26" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -1208,27 +1210,27 @@
     </row>
     <row r="2" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>20</v>
-      </c>
       <c r="E2" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactor: update imports and renaming
</commit_message>
<xml_diff>
--- a/tests/data/_schema/physical/car_dms_rules.xlsx
+++ b/tests/data/_schema/physical/car_dms_rules.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikola/Repos/neat/tests/data/_schema/physical/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndersAlbert\Projects\internal\neat\tests\data\_schema\physical\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DD1EA16-D174-8D4E-83E4-990FACD0DC4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B755191-25CE-4DB2-9E24-10C8DB53C273}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="42700" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -132,9 +132,6 @@
     <t>make</t>
   </si>
   <si>
-    <t>edge(type=Car.Manufacturer)</t>
-  </si>
-  <si>
     <t>Manufacturer</t>
   </si>
   <si>
@@ -244,6 +241,9 @@
   </si>
   <si>
     <t>http://purl.org/cognite/neat/data-model/verified/conceptual/sp_example_car/CarModel/1/Color/name</t>
+  </si>
+  <si>
+    <t>edge(type=make)</t>
   </si>
 </sst>
 </file>
@@ -253,7 +253,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -627,13 +627,13 @@
   <sheetViews>
     <sheetView zoomScale="285" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="26.5" customWidth="1"/>
+    <col min="2" max="2" width="26.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="15.6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -641,7 +641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="15.6">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -649,7 +649,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="15.6">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -657,7 +657,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="15.6">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -665,17 +665,17 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="15.6">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="15.6">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="15.6">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -683,7 +683,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="15.6">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
@@ -691,7 +691,7 @@
         <v>45695.809878616063</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="15.6">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
@@ -699,12 +699,12 @@
         <v>45695.809878616303</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" ht="15.6">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" ht="15.6">
       <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
@@ -720,24 +720,24 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O3" sqref="O3:O7"/>
+      <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="34.5" customWidth="1"/>
-    <col min="2" max="2" width="13.5" customWidth="1"/>
+    <col min="1" max="1" width="34.44140625" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" customWidth="1"/>
     <col min="3" max="4" width="13" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="27.5" customWidth="1"/>
+    <col min="5" max="5" width="27.44140625" customWidth="1"/>
     <col min="6" max="6" width="13" customWidth="1"/>
     <col min="7" max="11" width="13" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="18.5" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="18.44140625" hidden="1" customWidth="1"/>
     <col min="13" max="14" width="13" hidden="1" customWidth="1"/>
     <col min="15" max="15" width="94.6640625" customWidth="1"/>
     <col min="16" max="16" width="70" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" ht="25.8">
       <c r="A1" s="3" t="s">
         <v>16</v>
       </c>
@@ -756,7 +756,7 @@
       <c r="N1" s="4"/>
       <c r="O1" s="4"/>
     </row>
-    <row r="2" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="18">
       <c r="A2" s="5" t="s">
         <v>17</v>
       </c>
@@ -806,7 +806,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" ht="15.6">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -814,30 +814,30 @@
         <v>34</v>
       </c>
       <c r="E3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F3" t="s">
         <v>35</v>
-      </c>
-      <c r="F3" t="s">
-        <v>36</v>
       </c>
       <c r="I3" t="b">
         <v>1</v>
       </c>
       <c r="O3" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="P3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="15.6">
       <c r="A4" t="s">
         <v>33</v>
       </c>
       <c r="B4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" t="s">
         <v>38</v>
-      </c>
-      <c r="F4" t="s">
-        <v>39</v>
       </c>
       <c r="G4" t="b">
         <v>1</v>
@@ -852,27 +852,27 @@
         <v>33</v>
       </c>
       <c r="L4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O4" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="P4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="15.6">
       <c r="A5" t="s">
         <v>33</v>
       </c>
       <c r="B5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" t="s">
         <v>41</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>42</v>
-      </c>
-      <c r="F5" t="s">
-        <v>43</v>
       </c>
       <c r="G5" t="b">
         <v>1</v>
@@ -887,24 +887,24 @@
         <v>33</v>
       </c>
       <c r="L5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O5" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="P5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="15.6">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
       </c>
       <c r="F6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G6" t="b">
         <v>1</v>
@@ -916,27 +916,27 @@
         <v>0</v>
       </c>
       <c r="K6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L6" t="s">
         <v>8</v>
       </c>
       <c r="O6" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="P6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="15.6">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
       </c>
       <c r="F7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G7" t="b">
         <v>1</v>
@@ -948,16 +948,16 @@
         <v>0</v>
       </c>
       <c r="K7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L7" t="s">
         <v>8</v>
       </c>
       <c r="O7" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="P7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -975,17 +975,17 @@
       <selection pane="bottomLeft" activeCell="G3" sqref="G3:G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="19.5" customWidth="1"/>
+    <col min="1" max="1" width="19.44140625" customWidth="1"/>
     <col min="2" max="6" width="13" customWidth="1"/>
     <col min="7" max="7" width="79.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="70" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="25.8">
       <c r="A1" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -995,7 +995,7 @@
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
     </row>
-    <row r="2" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="18">
       <c r="A2" s="5" t="s">
         <v>17</v>
       </c>
@@ -1006,13 +1006,13 @@
         <v>20</v>
       </c>
       <c r="D2" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>50</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>51</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>31</v>
@@ -1021,7 +1021,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="15.6">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -1029,38 +1029,38 @@
         <v>1</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15.6">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F4" t="b">
         <v>1</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15.6">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F5" t="b">
         <v>1</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1078,15 +1078,15 @@
       <selection pane="bottomLeft" activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="24.5" customWidth="1"/>
+    <col min="1" max="1" width="24.44140625" customWidth="1"/>
     <col min="2" max="6" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="25.8">
       <c r="A1" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -1094,7 +1094,7 @@
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
     </row>
-    <row r="2" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="18">
       <c r="A2" s="5" t="s">
         <v>27</v>
       </c>
@@ -1108,25 +1108,25 @@
         <v>30</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1143,28 +1143,28 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="30.5" customWidth="1"/>
+    <col min="1" max="1" width="30.44140625" customWidth="1"/>
     <col min="2" max="4" width="13" customWidth="1"/>
     <col min="5" max="5" width="13" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="25.8">
       <c r="A1" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
     </row>
-    <row r="2" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="18">
       <c r="A2" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>58</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>59</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>19</v>
@@ -1190,28 +1190,28 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="19.5" customWidth="1"/>
+    <col min="1" max="1" width="19.44140625" customWidth="1"/>
     <col min="2" max="4" width="13" customWidth="1"/>
     <col min="5" max="5" width="13" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="25.8">
       <c r="A1" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
     </row>
-    <row r="2" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="18">
       <c r="A2" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>61</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>62</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>19</v>
@@ -1223,12 +1223,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" t="s">
         <v>63</v>
-      </c>
-      <c r="B3" t="s">
-        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactor: update imports and renamings
</commit_message>
<xml_diff>
--- a/tests/data/_schema/physical/car_dms_rules.xlsx
+++ b/tests/data/_schema/physical/car_dms_rules.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikola/Repos/neat/tests/data/_schema/physical/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndersAlbert\Projects\internal\neat\tests\data\_schema\physical\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DD1EA16-D174-8D4E-83E4-990FACD0DC4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B755191-25CE-4DB2-9E24-10C8DB53C273}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="42700" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -132,9 +132,6 @@
     <t>make</t>
   </si>
   <si>
-    <t>edge(type=Car.Manufacturer)</t>
-  </si>
-  <si>
     <t>Manufacturer</t>
   </si>
   <si>
@@ -244,6 +241,9 @@
   </si>
   <si>
     <t>http://purl.org/cognite/neat/data-model/verified/conceptual/sp_example_car/CarModel/1/Color/name</t>
+  </si>
+  <si>
+    <t>edge(type=make)</t>
   </si>
 </sst>
 </file>
@@ -253,7 +253,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -627,13 +627,13 @@
   <sheetViews>
     <sheetView zoomScale="285" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="26.5" customWidth="1"/>
+    <col min="2" max="2" width="26.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="15.6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -641,7 +641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="15.6">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -649,7 +649,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="15.6">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -657,7 +657,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="15.6">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -665,17 +665,17 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="15.6">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="15.6">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="15.6">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -683,7 +683,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="15.6">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
@@ -691,7 +691,7 @@
         <v>45695.809878616063</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="15.6">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
@@ -699,12 +699,12 @@
         <v>45695.809878616303</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" ht="15.6">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" ht="15.6">
       <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
@@ -720,24 +720,24 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O3" sqref="O3:O7"/>
+      <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="34.5" customWidth="1"/>
-    <col min="2" max="2" width="13.5" customWidth="1"/>
+    <col min="1" max="1" width="34.44140625" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" customWidth="1"/>
     <col min="3" max="4" width="13" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="27.5" customWidth="1"/>
+    <col min="5" max="5" width="27.44140625" customWidth="1"/>
     <col min="6" max="6" width="13" customWidth="1"/>
     <col min="7" max="11" width="13" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="18.5" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="18.44140625" hidden="1" customWidth="1"/>
     <col min="13" max="14" width="13" hidden="1" customWidth="1"/>
     <col min="15" max="15" width="94.6640625" customWidth="1"/>
     <col min="16" max="16" width="70" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" ht="25.8">
       <c r="A1" s="3" t="s">
         <v>16</v>
       </c>
@@ -756,7 +756,7 @@
       <c r="N1" s="4"/>
       <c r="O1" s="4"/>
     </row>
-    <row r="2" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="18">
       <c r="A2" s="5" t="s">
         <v>17</v>
       </c>
@@ -806,7 +806,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" ht="15.6">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -814,30 +814,30 @@
         <v>34</v>
       </c>
       <c r="E3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F3" t="s">
         <v>35</v>
-      </c>
-      <c r="F3" t="s">
-        <v>36</v>
       </c>
       <c r="I3" t="b">
         <v>1</v>
       </c>
       <c r="O3" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="P3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="15.6">
       <c r="A4" t="s">
         <v>33</v>
       </c>
       <c r="B4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" t="s">
         <v>38</v>
-      </c>
-      <c r="F4" t="s">
-        <v>39</v>
       </c>
       <c r="G4" t="b">
         <v>1</v>
@@ -852,27 +852,27 @@
         <v>33</v>
       </c>
       <c r="L4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O4" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="P4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="15.6">
       <c r="A5" t="s">
         <v>33</v>
       </c>
       <c r="B5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" t="s">
         <v>41</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>42</v>
-      </c>
-      <c r="F5" t="s">
-        <v>43</v>
       </c>
       <c r="G5" t="b">
         <v>1</v>
@@ -887,24 +887,24 @@
         <v>33</v>
       </c>
       <c r="L5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O5" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="P5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="15.6">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
       </c>
       <c r="F6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G6" t="b">
         <v>1</v>
@@ -916,27 +916,27 @@
         <v>0</v>
       </c>
       <c r="K6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L6" t="s">
         <v>8</v>
       </c>
       <c r="O6" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="P6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="15.6">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
       </c>
       <c r="F7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G7" t="b">
         <v>1</v>
@@ -948,16 +948,16 @@
         <v>0</v>
       </c>
       <c r="K7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L7" t="s">
         <v>8</v>
       </c>
       <c r="O7" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="P7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -975,17 +975,17 @@
       <selection pane="bottomLeft" activeCell="G3" sqref="G3:G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="19.5" customWidth="1"/>
+    <col min="1" max="1" width="19.44140625" customWidth="1"/>
     <col min="2" max="6" width="13" customWidth="1"/>
     <col min="7" max="7" width="79.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="70" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="25.8">
       <c r="A1" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -995,7 +995,7 @@
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
     </row>
-    <row r="2" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="18">
       <c r="A2" s="5" t="s">
         <v>17</v>
       </c>
@@ -1006,13 +1006,13 @@
         <v>20</v>
       </c>
       <c r="D2" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>50</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>51</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>31</v>
@@ -1021,7 +1021,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="15.6">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -1029,38 +1029,38 @@
         <v>1</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15.6">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F4" t="b">
         <v>1</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15.6">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F5" t="b">
         <v>1</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1078,15 +1078,15 @@
       <selection pane="bottomLeft" activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="24.5" customWidth="1"/>
+    <col min="1" max="1" width="24.44140625" customWidth="1"/>
     <col min="2" max="6" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="25.8">
       <c r="A1" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -1094,7 +1094,7 @@
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
     </row>
-    <row r="2" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="18">
       <c r="A2" s="5" t="s">
         <v>27</v>
       </c>
@@ -1108,25 +1108,25 @@
         <v>30</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1143,28 +1143,28 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="30.5" customWidth="1"/>
+    <col min="1" max="1" width="30.44140625" customWidth="1"/>
     <col min="2" max="4" width="13" customWidth="1"/>
     <col min="5" max="5" width="13" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="25.8">
       <c r="A1" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
     </row>
-    <row r="2" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="18">
       <c r="A2" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>58</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>59</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>19</v>
@@ -1190,28 +1190,28 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="19.5" customWidth="1"/>
+    <col min="1" max="1" width="19.44140625" customWidth="1"/>
     <col min="2" max="4" width="13" customWidth="1"/>
     <col min="5" max="5" width="13" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="25.8">
       <c r="A1" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
     </row>
-    <row r="2" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="18">
       <c r="A2" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>61</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>62</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>19</v>
@@ -1223,12 +1223,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" t="s">
         <v>63</v>
-      </c>
-      <c r="B3" t="s">
-        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Neat 969 rename dms to physical data model (#1195)
</commit_message>
<xml_diff>
--- a/tests/data/_schema/physical/car_dms_rules.xlsx
+++ b/tests/data/_schema/physical/car_dms_rules.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikola/Repos/neat/tests/data/_schema/physical/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DD1EA16-D174-8D4E-83E4-990FACD0DC4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F87C31E1-F3AA-7549-8BB1-7B9DC6D96D2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="42700" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="42700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -72,9 +72,6 @@
     <t>sourceId</t>
   </si>
   <si>
-    <t>logical</t>
-  </si>
-  <si>
     <t>Definition of Properties per Class</t>
   </si>
   <si>
@@ -120,9 +117,6 @@
     <t>Constraint</t>
   </si>
   <si>
-    <t>Logical</t>
-  </si>
-  <si>
     <t>Neat ID</t>
   </si>
   <si>
@@ -244,6 +238,12 @@
   </si>
   <si>
     <t>http://purl.org/cognite/neat/data-model/verified/conceptual/sp_example_car/CarModel/1/Color/name</t>
+  </si>
+  <si>
+    <t>Conceptual</t>
+  </si>
+  <si>
+    <t>conceptual</t>
   </si>
 </sst>
 </file>
@@ -625,7 +625,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView zoomScale="285" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="285" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -706,7 +708,7 @@
     </row>
     <row r="11" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>15</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -718,9 +720,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+    <sheetView zoomScale="125" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O3" sqref="O3:O7"/>
+      <selection pane="bottomLeft" activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -739,7 +741,7 @@
   <sheetData>
     <row r="1" spans="1:16" ht="26" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -758,86 +760,86 @@
     </row>
     <row r="2" spans="1:16" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="I2" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="J2" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="K2" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="L2" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="M2" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="N2" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="O2" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="P2" s="5" t="s">
         <v>30</v>
-      </c>
-      <c r="O2" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="P2" s="5" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" t="s">
         <v>33</v>
       </c>
-      <c r="B3" t="s">
+      <c r="F3" t="s">
         <v>34</v>
-      </c>
-      <c r="E3" t="s">
-        <v>35</v>
-      </c>
-      <c r="F3" t="s">
-        <v>36</v>
       </c>
       <c r="I3" t="b">
         <v>1</v>
       </c>
       <c r="O3" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="P3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G4" t="b">
         <v>1</v>
@@ -849,30 +851,30 @@
         <v>0</v>
       </c>
       <c r="K4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="L4" t="s">
+        <v>36</v>
+      </c>
+      <c r="O4" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="P4" t="s">
         <v>38</v>
-      </c>
-      <c r="O4" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="P4" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" t="s">
         <v>41</v>
-      </c>
-      <c r="E5" t="s">
-        <v>42</v>
-      </c>
-      <c r="F5" t="s">
-        <v>43</v>
       </c>
       <c r="G5" t="b">
         <v>1</v>
@@ -884,27 +886,27 @@
         <v>0</v>
       </c>
       <c r="K5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="L5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="O5" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="P5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
       </c>
       <c r="F6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G6" t="b">
         <v>1</v>
@@ -916,27 +918,27 @@
         <v>0</v>
       </c>
       <c r="K6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="L6" t="s">
         <v>8</v>
       </c>
       <c r="O6" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="P6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
       </c>
       <c r="F7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G7" t="b">
         <v>1</v>
@@ -948,16 +950,16 @@
         <v>0</v>
       </c>
       <c r="K7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="L7" t="s">
         <v>8</v>
       </c>
       <c r="O7" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="P7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -972,7 +974,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G3" sqref="G3:G5"/>
+      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -985,7 +987,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="26" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -997,70 +999,70 @@
     </row>
     <row r="2" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>20</v>
-      </c>
       <c r="D2" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>51</v>
-      </c>
       <c r="G2" s="5" t="s">
-        <v>31</v>
+        <v>71</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F3" t="b">
         <v>1</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F4" t="b">
         <v>1</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F5" t="b">
         <v>1</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1086,7 +1088,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="26" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -1096,37 +1098,37 @@
     </row>
     <row r="2" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>20</v>
-      </c>
       <c r="D2" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>30</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1152,7 +1154,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="26" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -1161,19 +1163,19 @@
     </row>
     <row r="2" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>20</v>
-      </c>
       <c r="E2" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1199,7 +1201,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="26" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -1208,27 +1210,27 @@
     </row>
     <row r="2" spans="1:5" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>20</v>
-      </c>
       <c r="E2" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tests: updated test data
</commit_message>
<xml_diff>
--- a/tests/data/_schema/physical/car_dms_rules.xlsx
+++ b/tests/data/_schema/physical/car_dms_rules.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikola/Repos/neat/tests/data/_schema/physical/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndersAlbert\Projects\main\neat\tests\data\_schema\physical\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F87C31E1-F3AA-7549-8BB1-7B9DC6D96D2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{713AA20B-B3DB-4AE7-84B9-BC30EEC1738C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="42700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -126,9 +126,6 @@
     <t>make</t>
   </si>
   <si>
-    <t>edge(type=Car.Manufacturer)</t>
-  </si>
-  <si>
     <t>Manufacturer</t>
   </si>
   <si>
@@ -244,6 +241,9 @@
   </si>
   <si>
     <t>conceptual</t>
+  </si>
+  <si>
+    <t>edge(type=make)</t>
   </si>
 </sst>
 </file>
@@ -253,7 +253,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -625,17 +625,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="285" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView zoomScale="285" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="26.5" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="15.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -643,7 +643,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="15.75">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -651,7 +651,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="15.75">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -659,7 +659,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="15.75">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -667,17 +667,17 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="15.75">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="15.75">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="15.75">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -685,7 +685,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="15.75">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
@@ -693,7 +693,7 @@
         <v>45695.809878616063</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="15.75">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
@@ -701,14 +701,14 @@
         <v>45695.809878616303</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" ht="15.75">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" ht="15.75">
       <c r="A11" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -720,26 +720,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P7"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O3" sqref="O3"/>
+      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="34.5" customWidth="1"/>
-    <col min="2" max="2" width="13.5" customWidth="1"/>
+    <col min="1" max="1" width="34.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" customWidth="1"/>
     <col min="3" max="4" width="13" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="27.5" customWidth="1"/>
+    <col min="5" max="5" width="27.42578125" customWidth="1"/>
     <col min="6" max="6" width="13" customWidth="1"/>
     <col min="7" max="11" width="13" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="18.5" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="18.42578125" hidden="1" customWidth="1"/>
     <col min="13" max="14" width="13" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="94.6640625" customWidth="1"/>
+    <col min="15" max="15" width="94.7109375" customWidth="1"/>
     <col min="16" max="16" width="70" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" ht="26.25">
       <c r="A1" s="3" t="s">
         <v>15</v>
       </c>
@@ -758,7 +758,7 @@
       <c r="N1" s="4"/>
       <c r="O1" s="4"/>
     </row>
-    <row r="2" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="18.75">
       <c r="A2" s="5" t="s">
         <v>16</v>
       </c>
@@ -802,13 +802,13 @@
         <v>29</v>
       </c>
       <c r="O2" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="P2" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" ht="15.75">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -816,30 +816,30 @@
         <v>32</v>
       </c>
       <c r="E3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F3" t="s">
         <v>33</v>
-      </c>
-      <c r="F3" t="s">
-        <v>34</v>
       </c>
       <c r="I3" t="b">
         <v>1</v>
       </c>
       <c r="O3" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="P3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="15.75">
       <c r="A4" t="s">
         <v>31</v>
       </c>
       <c r="B4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F4" t="s">
         <v>36</v>
-      </c>
-      <c r="F4" t="s">
-        <v>37</v>
       </c>
       <c r="G4" t="b">
         <v>1</v>
@@ -854,27 +854,27 @@
         <v>31</v>
       </c>
       <c r="L4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="O4" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="P4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="15.75">
       <c r="A5" t="s">
         <v>31</v>
       </c>
       <c r="B5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" t="s">
         <v>39</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>40</v>
-      </c>
-      <c r="F5" t="s">
-        <v>41</v>
       </c>
       <c r="G5" t="b">
         <v>1</v>
@@ -889,24 +889,24 @@
         <v>31</v>
       </c>
       <c r="L5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O5" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="P5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="15.75">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
       </c>
       <c r="F6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G6" t="b">
         <v>1</v>
@@ -918,27 +918,27 @@
         <v>0</v>
       </c>
       <c r="K6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L6" t="s">
         <v>8</v>
       </c>
       <c r="O6" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="P6" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="15.75">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
       </c>
       <c r="F7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G7" t="b">
         <v>1</v>
@@ -950,16 +950,16 @@
         <v>0</v>
       </c>
       <c r="K7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L7" t="s">
         <v>8</v>
       </c>
       <c r="O7" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="P7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -977,17 +977,17 @@
       <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.5" customWidth="1"/>
+    <col min="1" max="1" width="19.42578125" customWidth="1"/>
     <col min="2" max="6" width="13" customWidth="1"/>
-    <col min="7" max="7" width="79.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="79.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="70" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="26.25">
       <c r="A1" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -997,7 +997,7 @@
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
     </row>
-    <row r="2" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="18.75">
       <c r="A2" s="5" t="s">
         <v>16</v>
       </c>
@@ -1008,22 +1008,22 @@
         <v>19</v>
       </c>
       <c r="D2" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="F2" s="5" t="s">
-        <v>49</v>
-      </c>
       <c r="G2" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H2" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="15.75">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -1031,38 +1031,38 @@
         <v>1</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15.75">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F4" t="b">
         <v>1</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15.75">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F5" t="b">
         <v>1</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1080,15 +1080,15 @@
       <selection pane="bottomLeft" activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="24.5" customWidth="1"/>
+    <col min="1" max="1" width="24.42578125" customWidth="1"/>
     <col min="2" max="6" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="26.25">
       <c r="A1" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -1096,7 +1096,7 @@
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
     </row>
-    <row r="2" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="18.75">
       <c r="A2" s="5" t="s">
         <v>26</v>
       </c>
@@ -1110,25 +1110,25 @@
         <v>29</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1145,28 +1145,28 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="30.5" customWidth="1"/>
+    <col min="1" max="1" width="30.42578125" customWidth="1"/>
     <col min="2" max="4" width="13" customWidth="1"/>
     <col min="5" max="5" width="13" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="26.25">
       <c r="A1" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
     </row>
-    <row r="2" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="18.75">
       <c r="A2" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>56</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>57</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>18</v>
@@ -1192,28 +1192,28 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.5" customWidth="1"/>
+    <col min="1" max="1" width="19.42578125" customWidth="1"/>
     <col min="2" max="4" width="13" customWidth="1"/>
     <col min="5" max="5" width="13" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="26.25">
       <c r="A1" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
     </row>
-    <row r="2" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="18.75">
       <c r="A2" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>59</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>60</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>18</v>
@@ -1225,12 +1225,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" t="s">
         <v>61</v>
-      </c>
-      <c r="B3" t="s">
-        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>